<commit_message>
adding DDT - reading data from Excel and CSV files
</commit_message>
<xml_diff>
--- a/testdata/excel_file.xlsx
+++ b/testdata/excel_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saidgaforov/PycharmProjects/PythonSeleniumFramework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE56844-1E84-4C45-8FD8-66EF2B6C41D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5C7B67-D6E2-0245-A9D2-02228A609D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0F8E35D1-249F-F14B-B589-1A780CB102AA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>depart_from</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>LAS</t>
+  </si>
+  <si>
+    <t>10/15/2023</t>
+  </si>
+  <si>
+    <t>10/20/2023</t>
+  </si>
+  <si>
+    <t>11/03/2023</t>
   </si>
 </sst>
 </file>
@@ -102,7 +111,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +429,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,8 +461,8 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
-        <v>45179</v>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -466,8 +475,8 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
-        <v>45184</v>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -480,8 +489,8 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
-        <v>45206</v>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>

</xml_diff>